<commit_message>
ADD Homework to Seminar-02
</commit_message>
<xml_diff>
--- a/Seminar_02/Task_02.xlsx
+++ b/Seminar_02/Task_02.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YandexDisk\2_home\Learn_Programming\GeekBrains\Labs\Labs_GB\Databases\Seminars\Seminar_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C644AC48-3314-45C8-9AD6-125B66B69CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61487A-D78A-4D38-9AC6-9797F72488D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="1890" windowWidth="21600" windowHeight="10920" firstSheet="1" activeTab="1" xr2:uid="{D43C3157-60CC-4AA2-B380-DC5FD8CE980C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="7" xr2:uid="{D43C3157-60CC-4AA2-B380-DC5FD8CE980C}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
-    <sheet name="3" sheetId="2" r:id="rId2"/>
-    <sheet name="5" sheetId="3" r:id="rId3"/>
-    <sheet name="7" sheetId="4" r:id="rId4"/>
+    <sheet name="2" sheetId="5" r:id="rId2"/>
+    <sheet name="3" sheetId="2" r:id="rId3"/>
+    <sheet name="4" sheetId="6" r:id="rId4"/>
+    <sheet name="5" sheetId="3" r:id="rId5"/>
+    <sheet name="6" sheetId="7" r:id="rId6"/>
+    <sheet name="7" sheetId="4" r:id="rId7"/>
+    <sheet name="8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="34">
   <si>
     <t>Иванов И. И.</t>
   </si>
@@ -84,6 +88,60 @@
   </si>
   <si>
     <t>RIGHT JOIN Люди, Телефоны ON  id = Чей телефон</t>
+  </si>
+  <si>
+    <t>INNER JOIN Люди, Адреса ON  id = Чей адрес</t>
+  </si>
+  <si>
+    <t>Можга</t>
+  </si>
+  <si>
+    <t>Место рождения</t>
+  </si>
+  <si>
+    <t>Казань</t>
+  </si>
+  <si>
+    <t>По прописке</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Рабочий</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
+  </si>
+  <si>
+    <t>Белгород</t>
+  </si>
+  <si>
+    <t>LEFT JOIN Люди, Адреса ON  id = Чей адрес</t>
+  </si>
+  <si>
+    <t>RIGHT JOIN Люди, Адреса ON  id = Чей адрес</t>
+  </si>
+  <si>
+    <t>Уфа</t>
+  </si>
+  <si>
+    <t>Сочи</t>
+  </si>
+  <si>
+    <t>Киров</t>
+  </si>
+  <si>
+    <t>Владивосток</t>
+  </si>
+  <si>
+    <t>Рязань</t>
+  </si>
+  <si>
+    <t>Хабаровск</t>
+  </si>
+  <si>
+    <t>FULL JOIN Люди, Адреса ON  id = Чей адрес</t>
   </si>
 </sst>
 </file>
@@ -485,7 +543,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F11"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,11 +744,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A297C6C-9ECC-4320-809B-62D0BDC934EC}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>37152</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30429</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>35936</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A476F3F-13DE-4900-9C18-D6B66156DC1C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,7 +1115,173 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D23184E-DA56-4573-A893-8B55F4E93DE2}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>37152</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30429</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>35936</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43972</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996B6B21-17AB-4E8C-9B8E-EEDA819CB1FE}">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -1215,7 +1586,273 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E74FAE-851A-4350-B2CC-FAD6B8C7F5BA}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>37152</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30429</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>35936</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF406DC-7109-446C-93B6-4FBB45E53681}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -1538,4 +2175,291 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD09241-B127-48F8-BAE5-8FCBDBF0A15E}">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32916</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>37152</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30429</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>35936</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43972</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>